<commit_message>
updating UC documentation files
</commit_message>
<xml_diff>
--- a/documentation/function_points.xlsx
+++ b/documentation/function_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strau\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D3B3BFA-4C64-45FC-9852-A07E13CAB557}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6406DAE-A599-47B5-AB1C-5C44ED108D89}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="86">
   <si>
     <t>Estimated time</t>
   </si>
@@ -259,16 +259,31 @@
     <t>24h 25min</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
     <t>48h 55min</t>
   </si>
   <si>
-    <t>Sum Min / Sum Points</t>
-  </si>
-  <si>
     <t>Spent Time (min)</t>
+  </si>
+  <si>
+    <t>Change Account Password</t>
+  </si>
+  <si>
+    <t>Change Account Email</t>
+  </si>
+  <si>
+    <t>-3h 42m</t>
+  </si>
+  <si>
+    <t>6h 37m</t>
+  </si>
+  <si>
+    <t>2h 29m</t>
+  </si>
+  <si>
+    <t>Sum Spent Time / Sum Points</t>
+  </si>
+  <si>
+    <t>Sum of old Ucs</t>
   </si>
 </sst>
 </file>
@@ -278,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -337,8 +352,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,8 +389,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9B9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -489,17 +528,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -542,9 +570,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -555,10 +581,45 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -568,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -615,12 +676,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -629,27 +684,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -661,6 +702,44 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -668,6 +747,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9B9B"/>
+      <color rgb="FFFFB7B7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -700,11 +785,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -732,11 +817,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -768,28 +853,280 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
               <a:noFill/>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="6"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:shade val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-6846-4BCB-B475-AE5FCE3B6C5C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:shade val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-6846-4BCB-B475-AE5FCE3B6C5C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:shade val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-6846-4BCB-B475-AE5FCE3B6C5C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:shade val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-6846-4BCB-B475-AE5FCE3B6C5C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:shade val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6846-4BCB-B475-AE5FCE3B6C5C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:shade val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6846-4BCB-B475-AE5FCE3B6C5C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:shade val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6846-4BCB-B475-AE5FCE3B6C5C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:shade val="95000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-6846-4BCB-B475-AE5FCE3B6C5C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:trendline>
             <c:spPr>
               <a:ln w="9525" cap="rnd">
@@ -815,9 +1152,9 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx1">
+                          <a:schemeClr val="dk1">
                             <a:lumMod val="65000"/>
                             <a:lumOff val="35000"/>
                           </a:schemeClr>
@@ -828,10 +1165,9 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                      <a:rPr lang="en-US"/>
                       <a:t>fp(time) = 0,0284 * time + 16,006</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" sz="1100"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -848,9 +1184,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
+                        <a:schemeClr val="dk1">
                           <a:lumMod val="65000"/>
                           <a:lumOff val="35000"/>
                         </a:schemeClr>
@@ -867,10 +1203,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabellenblatt1!$C$3:$C$7</c:f>
+              <c:f>Tabellenblatt1!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>846</c:v>
                 </c:pt>
@@ -886,17 +1222,26 @@
                 <c:pt idx="4">
                   <c:v>429</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>-222</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>149</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabellenblatt1!$D$3:$D$7</c:f>
+              <c:f>Tabellenblatt1!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>29.92</c:v>
+                  <c:v>25.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>64.239999999999995</c:v>
@@ -909,6 +1254,15 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>37.840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.239999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -942,7 +1296,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -959,9 +1313,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -994,9 +1348,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -1016,11 +1370,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1032,9 +1386,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -1062,7 +1416,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1079,9 +1433,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -1093,14 +1447,10 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Function</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> Points</a:t>
+                  <a:t>Function Points</a:t>
                 </a:r>
                 <a:br>
-                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:rPr lang="de-DE"/>
                 </a:br>
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
@@ -1119,9 +1469,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -1141,11 +1491,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1157,9 +1507,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -1177,7 +1527,21 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1194,7 +1558,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1259,43 +1623,43 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea mods="allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1308,7 +1672,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1323,12 +1687,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1359,49 +1723,66 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -1410,26 +1791,25 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -1453,19 +1833,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1484,13 +1865,14 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1502,13 +1884,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1520,9 +1903,9 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -1549,7 +1932,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1566,13 +1949,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1584,13 +1968,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1602,13 +1987,14 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1617,22 +2003,39 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1">
+              <a:alpha val="0"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1645,17 +2048,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1671,9 +2074,9 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1687,12 +2090,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1716,12 +2119,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -1734,14 +2137,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:upBar>
   <cs:valueAxis>
@@ -1749,23 +2144,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -1782,16 +2177,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1223121</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2666999</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2118,13 +2513,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
@@ -2137,157 +2532,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="E1" s="36"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" spans="1:10" ht="15">
+      <c r="A3" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="35">
+        <v>846</v>
+      </c>
+      <c r="D3" s="42">
+        <v>25.52</v>
+      </c>
+      <c r="E3" s="43"/>
+    </row>
+    <row r="4" spans="1:10" ht="15">
+      <c r="A4" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="35">
+        <v>1559</v>
+      </c>
+      <c r="D4" s="42">
+        <v>64.239999999999995</v>
+      </c>
+      <c r="E4" s="43"/>
+    </row>
+    <row r="5" spans="1:10" ht="15">
+      <c r="A5" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="35">
+        <v>596</v>
+      </c>
+      <c r="D5" s="42">
+        <v>29.92</v>
+      </c>
+      <c r="E5" s="43"/>
+    </row>
+    <row r="6" spans="1:10" ht="15">
+      <c r="A6" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="35">
+        <v>203</v>
+      </c>
+      <c r="D6" s="42">
+        <v>21.12</v>
+      </c>
+      <c r="E6" s="43"/>
+    </row>
+    <row r="7" spans="1:10" ht="15">
+      <c r="A7" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="35">
+        <v>429</v>
+      </c>
+      <c r="D7" s="42">
+        <v>37.840000000000003</v>
+      </c>
+      <c r="E7" s="43"/>
+    </row>
+    <row r="8" spans="1:10" ht="15">
+      <c r="A8" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="46">
+        <v>-222</v>
+      </c>
+      <c r="D8" s="47">
+        <v>9.68</v>
+      </c>
+      <c r="E8" s="43"/>
+    </row>
+    <row r="9" spans="1:10" ht="15">
+      <c r="A9" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="47"/>
-    </row>
-    <row r="3" spans="1:10" ht="15">
-      <c r="A3" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="37">
-        <v>846</v>
-      </c>
-      <c r="D3" s="50">
-        <v>29.92</v>
-      </c>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="4" spans="1:10" ht="15">
-      <c r="A4" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="37">
-        <v>1559</v>
-      </c>
-      <c r="D4" s="50">
-        <v>64.239999999999995</v>
-      </c>
-      <c r="E4" s="51"/>
-    </row>
-    <row r="5" spans="1:10" ht="15">
-      <c r="A5" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="37">
-        <v>596</v>
-      </c>
-      <c r="D5" s="50">
-        <v>29.92</v>
-      </c>
-      <c r="E5" s="51"/>
-    </row>
-    <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="37">
-        <v>203</v>
-      </c>
-      <c r="D6" s="50">
-        <v>21.12</v>
-      </c>
-      <c r="E6" s="51"/>
-    </row>
-    <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="37">
-        <v>429</v>
-      </c>
-      <c r="D7" s="50">
-        <v>37.840000000000003</v>
-      </c>
-      <c r="E7" s="51"/>
-    </row>
-    <row r="8" spans="1:10" ht="15">
-      <c r="A8" s="42" t="s">
+      <c r="B9" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="35">
+        <v>397</v>
+      </c>
+      <c r="D9" s="42">
+        <v>27.28</v>
+      </c>
+      <c r="E9" s="43"/>
+    </row>
+    <row r="10" spans="1:10" ht="15">
+      <c r="A10" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="55">
+        <v>149</v>
+      </c>
+      <c r="D10" s="56">
+        <v>20.239999999999998</v>
+      </c>
+      <c r="E10" s="43"/>
+    </row>
+    <row r="11" spans="1:10" ht="12.75"/>
+    <row r="12" spans="1:10" ht="15">
+      <c r="A12" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="35">
+      <c r="C12" s="60">
         <f>SUM(C3:C7)</f>
         <v>3633</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D12" s="61">
         <f>SUM(D3:D7)</f>
-        <v>183.04</v>
-      </c>
-      <c r="E8" s="51"/>
-    </row>
-    <row r="9" spans="1:10" ht="15">
-      <c r="A9" s="38"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="51"/>
-    </row>
-    <row r="10" spans="1:10" thickBot="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="51"/>
-    </row>
-    <row r="11" spans="1:10" thickBot="1">
-      <c r="A11" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="46">
-        <f>C8/D8</f>
-        <v>19.84812062937063</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="24"/>
-    </row>
-    <row r="12" spans="1:10" ht="15">
-      <c r="A12" s="38"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="38"/>
-      <c r="B13" s="24"/>
+        <v>178.64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" thickBot="1">
+      <c r="A13" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="57">
+        <f>C12/D12</f>
+        <v>20.336990595611287</v>
+      </c>
       <c r="C13" s="25"/>
       <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A14" s="39"/>
+      <c r="A14" s="37"/>
     </row>
     <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="38"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="24"/>
       <c r="C15" s="25"/>
       <c r="D15" s="24"/>
@@ -3801,17 +4215,17 @@
       </c>
     </row>
     <row r="105" spans="4:5" ht="15.75" customHeight="1">
-      <c r="D105" s="53"/>
-      <c r="E105" s="53"/>
+      <c r="D105" s="45"/>
+      <c r="E105" s="45"/>
     </row>
     <row r="106" spans="4:5" ht="15.75" customHeight="1">
-      <c r="D106" s="52"/>
+      <c r="D106" s="44"/>
     </row>
     <row r="107" spans="4:5" ht="15.75" customHeight="1">
-      <c r="D107" s="52"/>
+      <c r="D107" s="44"/>
     </row>
     <row r="108" spans="4:5" ht="15.75" customHeight="1">
-      <c r="D108" s="52"/>
+      <c r="D108" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed misleading title ^DJ-132
</commit_message>
<xml_diff>
--- a/documentation/function_points.xlsx
+++ b/documentation/function_points.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="88">
   <si>
     <t>Estimated time</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>5h 50m</t>
+  </si>
+  <si>
+    <t>New Uc</t>
+  </si>
+  <si>
+    <t>Calculated Time</t>
   </si>
 </sst>
 </file>
@@ -966,7 +972,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabellenblatt1!$C$8:$C$10</c:f>
+              <c:f>Tabellenblatt1!$C$9:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -984,7 +990,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabellenblatt1!$D$8:$D$10</c:f>
+              <c:f>Tabellenblatt1!$D$9:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1755,7 +1761,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1673469</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>5862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2081,7 +2087,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M108"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -2101,10 +2107,10 @@
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1">
+    <row r="2" spans="1:5" ht="18" customHeight="1">
       <c r="A2" s="62" t="s">
         <v>74</v>
       </c>
@@ -2119,7 +2125,7 @@
       </c>
       <c r="E2" s="40"/>
     </row>
-    <row r="3" spans="1:10" ht="13.8">
+    <row r="3" spans="1:5" ht="13.8">
       <c r="A3" s="52" t="s">
         <v>2</v>
       </c>
@@ -2134,7 +2140,7 @@
       </c>
       <c r="E3" s="43"/>
     </row>
-    <row r="4" spans="1:10" ht="13.8">
+    <row r="4" spans="1:5" ht="13.8">
       <c r="A4" s="52" t="s">
         <v>3</v>
       </c>
@@ -2149,7 +2155,7 @@
       </c>
       <c r="E4" s="43"/>
     </row>
-    <row r="5" spans="1:10" ht="13.8">
+    <row r="5" spans="1:5" ht="13.8">
       <c r="A5" s="52" t="s">
         <v>4</v>
       </c>
@@ -2164,7 +2170,7 @@
       </c>
       <c r="E5" s="43"/>
     </row>
-    <row r="6" spans="1:10" ht="13.8">
+    <row r="6" spans="1:5" ht="13.8">
       <c r="A6" s="52" t="s">
         <v>6</v>
       </c>
@@ -2179,7 +2185,7 @@
       </c>
       <c r="E6" s="43"/>
     </row>
-    <row r="7" spans="1:10" ht="13.8">
+    <row r="7" spans="1:5" ht="13.8">
       <c r="A7" s="52" t="s">
         <v>8</v>
       </c>
@@ -2194,166 +2200,146 @@
       </c>
       <c r="E7" s="43"/>
     </row>
-    <row r="8" spans="1:10" ht="13.8">
-      <c r="A8" s="50" t="s">
+    <row r="8" spans="1:5" ht="13.8">
+      <c r="A8" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.8">
+      <c r="A9" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B9" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="46">
-        <f>1/0.043*D8</f>
+      <c r="C9" s="46">
+        <f>1/0.043*D9</f>
         <v>225.11627906976744</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D9" s="47">
         <v>9.68</v>
       </c>
-      <c r="E8" s="43"/>
-    </row>
-    <row r="9" spans="1:10" ht="13.8">
-      <c r="A9" s="51" t="s">
+      <c r="E9" s="43"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.8">
+      <c r="A10" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B10" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="46">
-        <f t="shared" ref="C9:C10" si="0">1/0.043*D9</f>
+      <c r="C10" s="46">
+        <f t="shared" ref="C10:C11" si="0">1/0.043*D10</f>
         <v>634.41860465116292</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D10" s="42">
         <v>27.28</v>
       </c>
-      <c r="E9" s="43"/>
-    </row>
-    <row r="10" spans="1:10" ht="13.8">
-      <c r="A10" s="53" t="s">
+      <c r="E10" s="43"/>
+    </row>
+    <row r="11" spans="1:5" ht="13.8">
+      <c r="A11" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B11" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C11" s="46">
         <f t="shared" si="0"/>
         <v>470.69767441860466</v>
       </c>
-      <c r="D10" s="55">
+      <c r="D11" s="55">
         <v>20.239999999999998</v>
       </c>
-      <c r="E10" s="43"/>
-    </row>
-    <row r="11" spans="1:10" ht="13.2"/>
-    <row r="12" spans="1:10" ht="13.8">
-      <c r="A12" s="57" t="s">
+      <c r="E11" s="43"/>
+    </row>
+    <row r="12" spans="1:5" ht="13.2"/>
+    <row r="13" spans="1:5" ht="13.8">
+      <c r="A13" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B13" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="59">
+      <c r="C13" s="59">
         <f>SUM(C3:C7)</f>
         <v>3633</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D13" s="60">
         <f>SUM(D3:D7)</f>
         <v>178.64</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.4" thickBot="1">
-      <c r="A13" s="61" t="s">
+    <row r="14" spans="1:5" ht="14.4" thickBot="1">
+      <c r="A14" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="56">
-        <f>C12/D12</f>
+      <c r="B14" s="56">
+        <f>C13/D13</f>
         <v>20.336990595611287</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="24"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A14" s="37"/>
-    </row>
-    <row r="15" spans="1:10" ht="13.8">
-      <c r="A15" s="36"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.6">
-      <c r="A16" s="1" t="s">
+      <c r="C14" s="25"/>
+      <c r="D14" s="24"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A15" s="37"/>
+    </row>
+    <row r="16" spans="1:5" ht="13.8">
+      <c r="A16" s="36"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.6">
+      <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="G17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="13.2">
-      <c r="A17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="7">
-        <v>4</v>
-      </c>
-      <c r="D17" s="7">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="1:13" ht="13.2">
       <c r="A18" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D18" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>17</v>
@@ -2366,21 +2352,22 @@
         <v>18</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>18</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="M18" s="33"/>
     </row>
     <row r="19" spans="1:13" ht="13.2">
-      <c r="A19" s="12" t="s">
-        <v>23</v>
+      <c r="A19" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="7">
         <v>0</v>
@@ -2396,149 +2383,149 @@
         <v>18</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="13.2">
-      <c r="A20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="7">
-        <v>3</v>
+      <c r="A20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C20" s="7">
-        <v>4</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="13.2">
+      <c r="A21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7">
+        <v>4</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="7">
+        <v>2</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I21" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="13.2">
-      <c r="A21" s="13" t="s">
+      <c r="J21" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="13.2">
+      <c r="A22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="14">
-        <v>1</v>
-      </c>
-      <c r="C21" s="14">
+      <c r="B22" s="14">
+        <v>1</v>
+      </c>
+      <c r="C22" s="14">
         <v>4</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="14" t="s">
+      <c r="D22" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="14">
-        <v>1</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16" t="s">
+      <c r="F22" s="14">
+        <v>1</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I22" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.6">
-      <c r="A23" s="1" t="s">
+      <c r="J22" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.6">
+      <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="3" t="s">
+      <c r="G24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="13.2">
-      <c r="A24" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="7">
-        <v>5</v>
-      </c>
-      <c r="D24" s="7">
-        <v>2</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="7">
-        <v>2</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="13.2">
       <c r="A25" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D25" s="7">
         <v>2</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F25" s="7">
         <v>2</v>
@@ -2547,181 +2534,181 @@
       <c r="H25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="19" t="s">
-        <v>18</v>
+      <c r="I25" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="13.2">
       <c r="A26" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="19" t="s">
         <v>18</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.2">
       <c r="A27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="7">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C27" s="7">
-        <v>7</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="13.2">
+      <c r="A28" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="7">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7">
+        <v>7</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="7">
+        <v>2</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="13.2">
-      <c r="A28" s="13" t="s">
+      <c r="I28" s="19"/>
+      <c r="J28" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="13.2">
+      <c r="A29" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B29" s="14">
         <v>4</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="14" t="s">
+      <c r="D29" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="14">
-        <v>1</v>
-      </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16" t="s">
+      <c r="F29" s="14">
+        <v>1</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I28" s="17" t="s">
+      <c r="I29" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="J28" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="13.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="1:13" ht="15.6">
-      <c r="A30" s="1" t="s">
+      <c r="J29" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="13.2">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.6">
+      <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="3" t="s">
+      <c r="G31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="13.2">
-      <c r="A31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="7">
-        <v>4</v>
-      </c>
-      <c r="D31" s="7">
-        <v>1</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="7">
-        <v>2</v>
-      </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.2">
       <c r="A32" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D32" s="7">
         <v>1</v>
@@ -2730,14 +2717,14 @@
         <v>17</v>
       </c>
       <c r="F32" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="19" t="s">
-        <v>18</v>
+      <c r="I32" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="J32" s="11" t="s">
         <v>39</v>
@@ -2745,13 +2732,13 @@
     </row>
     <row r="33" spans="1:10" ht="13.2">
       <c r="A33" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D33" s="7">
         <v>1</v>
@@ -2766,8 +2753,8 @@
       <c r="H33" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I33" s="10" t="s">
-        <v>40</v>
+      <c r="I33" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="J33" s="11" t="s">
         <v>39</v>
@@ -2775,141 +2762,141 @@
     </row>
     <row r="34" spans="1:10" ht="13.2">
       <c r="A34" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="7">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C34" s="7">
-        <v>5</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F34" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="13.2">
+      <c r="A35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="7">
+        <v>5</v>
+      </c>
+      <c r="C35" s="7">
+        <v>5</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="7">
+        <v>3</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I34" s="10" t="s">
+      <c r="I35" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J34" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="13.2">
-      <c r="A35" s="13" t="s">
+      <c r="J35" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="13.2">
+      <c r="A36" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B36" s="14">
         <v>0</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C36" s="14">
         <v>0</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="14" t="s">
+      <c r="D36" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F36" s="14">
         <v>0</v>
       </c>
-      <c r="G35" s="15"/>
-      <c r="H35" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="13.2">
-      <c r="A36" s="20"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.6">
-      <c r="A37" s="1" t="s">
+      <c r="G36" s="15"/>
+      <c r="H36" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="13.2">
+      <c r="A37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.6">
+      <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H37" s="3" t="s">
+      <c r="G38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="J38" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="13.2">
-      <c r="A38" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="7">
-        <v>2</v>
-      </c>
-      <c r="D38" s="7">
-        <v>1</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" s="7">
-        <v>1</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J38" s="11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="13.2">
       <c r="A39" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D39" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>17</v>
@@ -2919,27 +2906,27 @@
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="9" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="13.2">
       <c r="A40" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D40" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>17</v>
@@ -2952,149 +2939,149 @@
         <v>18</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J40" s="21" t="s">
-        <v>18</v>
+        <v>46</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="13.2">
       <c r="A41" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="7">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C41" s="7">
-        <v>5</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="13.2">
+      <c r="A42" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="7">
+        <v>3</v>
+      </c>
+      <c r="C42" s="7">
+        <v>5</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="7">
+        <v>2</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="I42" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="J41" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="13.2">
-      <c r="A42" s="13" t="s">
+      <c r="J42" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="13.2">
+      <c r="A43" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B43" s="14">
         <v>0</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C43" s="14">
         <v>0</v>
       </c>
-      <c r="D42" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="14" t="s">
+      <c r="D43" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F42" s="14">
+      <c r="F43" s="14">
         <v>0</v>
       </c>
-      <c r="G42" s="15"/>
-      <c r="H42" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J42" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="13.2">
-      <c r="A43" s="20"/>
-    </row>
-    <row r="44" spans="1:10" ht="15.6">
-      <c r="A44" s="1" t="s">
+      <c r="G43" s="15"/>
+      <c r="H43" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="13.2">
+      <c r="A44" s="20"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.6">
+      <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H44" s="3" t="s">
+      <c r="G45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J45" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="13.2">
-      <c r="A45" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="7">
-        <v>1</v>
-      </c>
-      <c r="D45" s="7">
-        <v>1</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F45" s="7">
-        <v>2</v>
-      </c>
-      <c r="G45" s="8"/>
-      <c r="H45" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J45" s="21" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="13.2">
       <c r="A46" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C46" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>17</v>
@@ -3107,7 +3094,7 @@
         <v>18</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="J46" s="21" t="s">
         <v>18</v>
@@ -3115,29 +3102,29 @@
     </row>
     <row r="47" spans="1:10" ht="13.2">
       <c r="A47" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C47" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D47" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F47" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I47" s="19" t="s">
-        <v>18</v>
+      <c r="I47" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="J47" s="21" t="s">
         <v>18</v>
@@ -3145,191 +3132,191 @@
     </row>
     <row r="48" spans="1:10" ht="13.2">
       <c r="A48" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="7">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C48" s="7">
-        <v>3</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F48" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="13.2">
+      <c r="A49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="7">
+        <v>3</v>
+      </c>
+      <c r="C49" s="7">
+        <v>3</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="7">
+        <v>3</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I48" s="10" t="s">
+      <c r="I49" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J48" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="13.2">
-      <c r="A49" s="13" t="s">
+      <c r="J49" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="13.2">
+      <c r="A50" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="14">
-        <v>1</v>
-      </c>
-      <c r="C49" s="14">
+      <c r="B50" s="14">
+        <v>1</v>
+      </c>
+      <c r="C50" s="14">
         <v>4</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" s="14" t="s">
+      <c r="D50" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F49" s="14">
-        <v>1</v>
-      </c>
-      <c r="G49" s="15"/>
-      <c r="H49" s="16" t="s">
+      <c r="F50" s="14">
+        <v>1</v>
+      </c>
+      <c r="G50" s="15"/>
+      <c r="H50" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I49" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J49" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="13.2">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="27"/>
-    </row>
-    <row r="51" spans="1:10" ht="14.4">
-      <c r="A51" s="29" t="s">
+      <c r="I50" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="13.2">
+      <c r="A51" s="26"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="27"/>
+    </row>
+    <row r="52" spans="1:10" ht="14.4">
+      <c r="A52" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="29"/>
-    </row>
-    <row r="53" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A53" s="1" t="s">
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="29"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H53" s="3" t="s">
+      <c r="G54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H54" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J53" s="5" t="s">
+      <c r="J54" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A54" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="7">
-        <v>3</v>
-      </c>
-      <c r="D54" s="7">
-        <v>1</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F54" s="7">
-        <v>0</v>
-      </c>
-      <c r="G54" s="8"/>
-      <c r="H54" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J54" s="21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1">
       <c r="A55" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C55" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D55" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F55" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55" s="8"/>
       <c r="H55" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J55" s="21" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1">
       <c r="A56" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C56" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D56" s="7">
         <v>0</v>
@@ -3338,14 +3325,14 @@
         <v>17</v>
       </c>
       <c r="F56" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I56" s="19" t="s">
-        <v>18</v>
+      <c r="I56" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="J56" s="21" t="s">
         <v>18</v>
@@ -3353,133 +3340,133 @@
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1">
       <c r="A57" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="7">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C57" s="7">
-        <v>5</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F57" s="7">
-        <v>1</v>
-      </c>
-      <c r="G57" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G57" s="8"/>
+      <c r="H57" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A58" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="7">
+        <v>1</v>
+      </c>
+      <c r="C58" s="7">
+        <v>5</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" s="7">
+        <v>1</v>
+      </c>
+      <c r="G58" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H57" s="9" t="s">
+      <c r="H58" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I57" s="10" t="s">
+      <c r="I58" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="J57" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A58" s="13" t="s">
+      <c r="J58" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A59" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B58" s="14">
+      <c r="B59" s="14">
         <v>0</v>
       </c>
-      <c r="C58" s="14">
+      <c r="C59" s="14">
         <v>0</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E58" s="14" t="s">
+      <c r="D59" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F58" s="14">
+      <c r="F59" s="14">
         <v>0</v>
       </c>
-      <c r="G58" s="32" t="s">
+      <c r="G59" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="H58" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I58" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J58" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A60" s="1" t="s">
+      <c r="H59" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A61" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H60" s="3" t="s">
+      <c r="G61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H61" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="I61" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J60" s="5" t="s">
+      <c r="J61" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A61" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="7">
-        <v>3</v>
-      </c>
-      <c r="D61" s="7">
-        <v>1</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F61" s="7">
-        <v>0</v>
-      </c>
-      <c r="G61" s="8"/>
-      <c r="H61" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J61" s="21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15.75" customHeight="1">
       <c r="A62" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>16</v>
@@ -3488,34 +3475,34 @@
         <v>3</v>
       </c>
       <c r="D62" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F62" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G62" s="8"/>
       <c r="H62" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="J62" s="21" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15.75" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C63" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D63" s="7">
         <v>0</v>
@@ -3524,14 +3511,14 @@
         <v>17</v>
       </c>
       <c r="F63" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G63" s="8"/>
       <c r="H63" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I63" s="19" t="s">
-        <v>18</v>
+      <c r="I63" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="J63" s="21" t="s">
         <v>18</v>
@@ -3539,133 +3526,133 @@
     </row>
     <row r="64" spans="1:10" ht="15.75" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B64" s="7">
-        <v>2</v>
+        <v>23</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C64" s="7">
-        <v>5</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="D64" s="7">
+        <v>0</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F64" s="7">
+        <v>0</v>
+      </c>
+      <c r="G64" s="8"/>
+      <c r="H64" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I64" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A65" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="7">
         <v>2</v>
       </c>
-      <c r="G64" s="31" t="s">
+      <c r="C65" s="7">
+        <v>5</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="7">
+        <v>2</v>
+      </c>
+      <c r="G65" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H64" s="9" t="s">
+      <c r="H65" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I64" s="10" t="s">
+      <c r="I65" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J64" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A65" s="13" t="s">
+      <c r="J65" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A66" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="14">
-        <v>1</v>
-      </c>
-      <c r="C65" s="14">
+      <c r="B66" s="14">
+        <v>1</v>
+      </c>
+      <c r="C66" s="14">
         <v>0</v>
       </c>
-      <c r="D65" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" s="14" t="s">
+      <c r="D66" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F65" s="14">
-        <v>1</v>
-      </c>
-      <c r="G65" s="32" t="s">
+      <c r="F66" s="14">
+        <v>1</v>
+      </c>
+      <c r="G66" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="H65" s="16" t="s">
+      <c r="H66" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I65" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J65" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A67" s="1" t="s">
+      <c r="I66" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J66" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A68" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G67" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H67" s="3" t="s">
+      <c r="G68" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H68" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="I68" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J67" s="5" t="s">
+      <c r="J68" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A68" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C68" s="7">
-        <v>2</v>
-      </c>
-      <c r="D68" s="7">
-        <v>1</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F68" s="7">
-        <v>1</v>
-      </c>
-      <c r="G68" s="8"/>
-      <c r="H68" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I68" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J68" s="21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1">
       <c r="A69" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>16</v>
@@ -3674,34 +3661,34 @@
         <v>2</v>
       </c>
       <c r="D69" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F69" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G69" s="8"/>
       <c r="H69" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J69" s="21" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1">
       <c r="A70" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C70" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D70" s="7">
         <v>0</v>
@@ -3710,14 +3697,14 @@
         <v>17</v>
       </c>
       <c r="F70" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G70" s="8"/>
       <c r="H70" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I70" s="19" t="s">
-        <v>18</v>
+      <c r="I70" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="J70" s="21" t="s">
         <v>18</v>
@@ -3725,86 +3712,116 @@
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B71" s="7">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C71" s="7">
-        <v>3</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="D71" s="7">
+        <v>0</v>
       </c>
       <c r="E71" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F71" s="7">
-        <v>1</v>
-      </c>
-      <c r="G71" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G71" s="8"/>
+      <c r="H71" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J71" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A72" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" s="7">
+        <v>1</v>
+      </c>
+      <c r="C72" s="7">
+        <v>3</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="7">
+        <v>1</v>
+      </c>
+      <c r="G72" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H71" s="9" t="s">
+      <c r="H72" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I71" s="10" t="s">
+      <c r="I72" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J71" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A72" s="13" t="s">
+      <c r="J72" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A73" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B72" s="14">
-        <v>1</v>
-      </c>
-      <c r="C72" s="14">
+      <c r="B73" s="14">
+        <v>1</v>
+      </c>
+      <c r="C73" s="14">
         <v>0</v>
       </c>
-      <c r="D72" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E72" s="14" t="s">
+      <c r="D73" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F72" s="14">
-        <v>1</v>
-      </c>
-      <c r="G72" s="32" t="s">
+      <c r="F73" s="14">
+        <v>1</v>
+      </c>
+      <c r="G73" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="H72" s="16" t="s">
+      <c r="H73" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I72" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="J72" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="105" spans="4:5" ht="15.75" customHeight="1">
-      <c r="D105" s="45"/>
-      <c r="E105" s="45"/>
+      <c r="I73" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="106" spans="4:5" ht="15.75" customHeight="1">
-      <c r="D106" s="44"/>
+      <c r="D106" s="45"/>
+      <c r="E106" s="45"/>
     </row>
     <row r="107" spans="4:5" ht="15.75" customHeight="1">
       <c r="D107" s="44"/>
     </row>
     <row r="108" spans="4:5" ht="15.75" customHeight="1">
       <c r="D108" s="44"/>
+    </row>
+    <row r="109" spans="4:5" ht="15.75" customHeight="1">
+      <c r="D109" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G58" twoDigitTextYear="1"/>
+    <ignoredError sqref="G59" twoDigitTextYear="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix misleading title ^DJ-132
</commit_message>
<xml_diff>
--- a/documentation/function_points.xlsx
+++ b/documentation/function_points.xlsx
@@ -285,10 +285,10 @@
     <t>5h 50m</t>
   </si>
   <si>
-    <t>New Uc</t>
-  </si>
-  <si>
-    <t>Calculated Time</t>
+    <t>New Use Case</t>
+  </si>
+  <si>
+    <t>Calculated Time (min)</t>
   </si>
 </sst>
 </file>
@@ -2090,14 +2090,14 @@
   <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" customWidth="1"/>
@@ -2200,15 +2200,15 @@
       </c>
       <c r="E7" s="43"/>
     </row>
-    <row r="8" spans="1:5" ht="13.8">
-      <c r="A8" s="52" t="s">
+    <row r="8" spans="1:5" ht="15.6">
+      <c r="A8" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="42"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="43"/>
     </row>
     <row r="9" spans="1:5" ht="13.8">

</xml_diff>